<commit_message>
oprava cteni databaze, pokrok v exportu...
</commit_message>
<xml_diff>
--- a/TRIMAZKON/Katalog_kamerového_vybavení.xlsx
+++ b/TRIMAZKON/Katalog_kamerového_vybavení.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,13 +25,59 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="25"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00ffffff"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <sz val="16"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001E90FF"/>
+        <bgColor rgb="001E90FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0032CD32"/>
+        <bgColor rgb="0032CD32"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF4500"/>
+        <bgColor rgb="00FF4500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00999999"/>
+        <bgColor rgb="00999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00636363"/>
+        <bgColor rgb="00636363"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +92,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -443,53 +520,513 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
+    <col width="50" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="50" customWidth="1" min="9" max="9"/>
+    <col width="50" customWidth="1" min="10" max="10"/>
+  </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
+    <row r="1" ht="35" customHeight="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Přehled kamerového vybavení</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="65" customHeight="1">
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Projekt: 
+Datum: 25.07.2024</t>
+        </is>
+      </c>
+    </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Stanice</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Kamera</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>Optika</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>Kontrolery</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="H3" s="3" t="n"/>
+      <c r="I3" s="3" t="inlineStr">
         <is>
           <t>Příslušenství</t>
         </is>
       </c>
+      <c r="J3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- popis inspekce- popis inspekce- popis inspekce- popis inspekce- popis inspekce- popis inspekce- popis inspekce- popis inspekce
+</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>FH-SC12</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kabel: FZ-VSB3 10M
+Kamera: FH kamera, velké rozlišení 12M pixel, barevný
+Kabel: příslušenství kamerových systémů, FH a FZ, kabel pro kameru, odolný ohybu, 10m
+http://industrial.omron.co.uk/en/search?q=G639
+</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>3Z4S-LE SV-3514H</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE SV-3514H
+Objektiv: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 25 mm, nejmenší vzdálenost 150mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+Alternativní: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 25 mm, nejmenší vzdálenost 150mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="inlineStr">
+        <is>
+          <t>FH-2050</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 1 (FH-2050)
+192.168.000.000
+</t>
+        </is>
+      </c>
+      <c r="I4" s="4" t="inlineStr">
+        <is>
+          <t>rozšíření kontroleru</t>
+        </is>
+      </c>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n"/>
+      <c r="B5" s="4" t="n"/>
+      <c r="C5" s="4" t="n"/>
+      <c r="D5" s="4" t="n"/>
+      <c r="E5" s="4" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="4" t="n"/>
+      <c r="H5" s="4" t="n"/>
+      <c r="I5" s="4" t="n"/>
+      <c r="J5" s="4" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="4" t="n"/>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="4" t="n"/>
+      <c r="E6" s="4" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="4" t="n"/>
+      <c r="H6" s="4" t="n"/>
+      <c r="I6" s="4" t="n"/>
+      <c r="J6" s="4" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="4" t="n"/>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="4" t="n"/>
+      <c r="E7" s="4" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="4" t="n"/>
+      <c r="H7" s="4" t="n"/>
+      <c r="I7" s="4" t="n"/>
+      <c r="J7" s="4" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="n"/>
+      <c r="B8" s="7" t="n"/>
+      <c r="C8" s="7" t="n"/>
+      <c r="D8" s="7" t="n"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr"/>
+      <c r="G8" s="7" t="n"/>
+      <c r="H8" s="7" t="n"/>
+      <c r="I8" s="7" t="n"/>
+      <c r="J8" s="7" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">22222222222222222
+</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>FH-SM</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kabel: FZ-VSLB3 5M
+Kamera: FH kamera, standardní rozlišení, monochromatický
+Kabel: příslušenství kamerových systémů, FH a FZ, kabel pro kameru, odolný ohybu, konektor úhlový, 5m
+</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>3Z4S-LE SV-7525H</t>
+        </is>
+      </c>
+      <c r="F9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE SV-2514H
+Objektiv: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 50 mm, nejmenší vzdálenost 300mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+Alternativní: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 16 mm, nejmenší vzdálenost 100mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="n"/>
+      <c r="H9" s="4" t="n"/>
+      <c r="I9" s="4" t="n"/>
+      <c r="J9" s="4" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="4" t="n"/>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="4" t="n"/>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>3Z4S-LE SV-10028H</t>
+        </is>
+      </c>
+      <c r="F10" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE SV-5014H
+Objektiv: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 75 mm, nejmenší vzdálenost 1200mm, světelnost 2,5 až zavřeno, maximální kompatiblní CCD čip 2/3" nebo 1", revize 1
+Alternativní: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 35 mm, nejmenší vzdálenost 200mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="n"/>
+      <c r="H10" s="4" t="n"/>
+      <c r="I10" s="4" t="n"/>
+      <c r="J10" s="4" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n"/>
+      <c r="B11" s="4" t="n"/>
+      <c r="C11" s="4" t="n"/>
+      <c r="D11" s="4" t="n"/>
+      <c r="E11" s="4" t="inlineStr"/>
+      <c r="F11" s="5" t="inlineStr"/>
+      <c r="G11" s="4" t="n"/>
+      <c r="H11" s="4" t="n"/>
+      <c r="I11" s="4" t="n"/>
+      <c r="J11" s="4" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n"/>
+      <c r="B12" s="4" t="n"/>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>FH-SM</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kabel: FZ-VSBX 10M
+Kamera: FH kamera, standardní rozlišení, monochromatický
+Kabel: Ultra bend resistant camera cable, 10 m
+</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>3Z4S-LE SV-5014H</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE VS-L10028/M42-10
+Objektiv: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 35 mm, nejmenší vzdálenost 200mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+Alternativní: Objektiv, ultra vysoké rozlišení, nízké zkreslení 16 mm pro 1/1" velik
+</t>
+        </is>
+      </c>
+      <c r="G12" s="9" t="inlineStr">
+        <is>
+          <t>FH-2050</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 2 (FH-2050)
+192.168.000.000
+</t>
+        </is>
+      </c>
+      <c r="I12" s="4" t="inlineStr">
+        <is>
+          <t>konzole</t>
+        </is>
+      </c>
+      <c r="J12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">adsfdffds
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n"/>
+      <c r="B13" s="4" t="n"/>
+      <c r="C13" s="4" t="n"/>
+      <c r="D13" s="4" t="n"/>
+      <c r="E13" s="4" t="inlineStr"/>
+      <c r="F13" s="5" t="inlineStr"/>
+      <c r="G13" s="4" t="n"/>
+      <c r="H13" s="4" t="n"/>
+      <c r="I13" s="4" t="n"/>
+      <c r="J13" s="4" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n"/>
+      <c r="B14" s="4" t="n"/>
+      <c r="C14" s="4" t="n"/>
+      <c r="D14" s="4" t="n"/>
+      <c r="E14" s="4" t="inlineStr"/>
+      <c r="F14" s="5" t="inlineStr"/>
+      <c r="G14" s="4" t="n"/>
+      <c r="H14" s="4" t="n"/>
+      <c r="I14" s="4" t="n"/>
+      <c r="J14" s="4" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="n"/>
+      <c r="B15" s="7" t="n"/>
+      <c r="C15" s="7" t="n"/>
+      <c r="D15" s="7" t="n"/>
+      <c r="E15" s="7" t="inlineStr"/>
+      <c r="F15" s="8" t="inlineStr"/>
+      <c r="G15" s="7" t="n"/>
+      <c r="H15" s="7" t="n"/>
+      <c r="I15" s="7" t="n"/>
+      <c r="J15" s="7" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- popis inspekce- popis inspekce- popis inspekce- popis inspekce
+</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="inlineStr">
+        <is>
+          <t>FH-SCX05</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kabel: FZ-VSB3 10M
+Kamera: FH kamera, vysokorychlostní, 5 Mpixel, C montáž, celková uzávěrka, barevný
+Kabel: příslušenství kamerových systémů, FH a FZ, kabel pro kameru, odolný ohybu, 10m
+http://industrial.omron.co.uk/en/search?q=G639
+</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="inlineStr">
+        <is>
+          <t>3Z4S-LE VS-HVA2524</t>
+        </is>
+      </c>
+      <c r="F16" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE VS-HVA3522
+Objektiv: Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 50 mm
+Alternativní: Příslušenství pro kamery, pro M42-montáž, prodlužovací kroužek, sada 5 kroužků (20, 10, 8, 2, 1 mm)
+</t>
+        </is>
+      </c>
+      <c r="G16" s="10" t="inlineStr">
+        <is>
+          <t>FH-2050</t>
+        </is>
+      </c>
+      <c r="H16" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 3 (FH-2050)
+192.168.000.000
+</t>
+        </is>
+      </c>
+      <c r="I16" s="4" t="inlineStr">
+        <is>
+          <t>kamera</t>
+        </is>
+      </c>
+      <c r="J16" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n"/>
+      <c r="B17" s="4" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="4" t="n"/>
+      <c r="E17" s="4" t="inlineStr"/>
+      <c r="F17" s="5" t="inlineStr"/>
+      <c r="G17" s="4" t="n"/>
+      <c r="H17" s="4" t="n"/>
+      <c r="I17" s="4" t="n"/>
+      <c r="J17" s="4" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="n"/>
+      <c r="B18" s="7" t="n"/>
+      <c r="C18" s="7" t="n"/>
+      <c r="D18" s="7" t="n"/>
+      <c r="E18" s="7" t="inlineStr"/>
+      <c r="F18" s="8" t="inlineStr"/>
+      <c r="G18" s="7" t="n"/>
+      <c r="H18" s="7" t="n"/>
+      <c r="I18" s="7" t="n"/>
+      <c r="J18" s="7" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
+          <t>Název staniceghggg</t>
+        </is>
+      </c>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- popis inspekce
+</t>
+        </is>
+      </c>
+      <c r="C19" s="4" t="inlineStr"/>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="inlineStr"/>
+      <c r="F19" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="n"/>
+      <c r="H19" s="4" t="n"/>
+      <c r="I19" s="4" t="n"/>
+      <c r="J19" s="4" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="n"/>
+      <c r="B20" s="11" t="n"/>
+      <c r="C20" s="11" t="n"/>
+      <c r="D20" s="11" t="n"/>
+      <c r="E20" s="11" t="n"/>
+      <c r="F20" s="11" t="n"/>
+      <c r="G20" s="11" t="n"/>
+      <c r="H20" s="11" t="n"/>
+      <c r="I20" s="11" t="n"/>
+      <c r="J20" s="11" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:A2"/>
+  <mergeCells count="30">
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
     <mergeCell ref="B1:J1"/>
-    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C9:C11"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B2:J2"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
dodelani exportu xlsm, zvysena kapacita komponent, warning pri ukladani xml
</commit_message>
<xml_diff>
--- a/TRIMAZKON/Katalog_kamerového_vybavení.xlsx
+++ b/TRIMAZKON/Katalog_kamerového_vybavení.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -39,10 +39,14 @@
       <sz val="20"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -51,8 +55,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00999999"/>
-        <bgColor rgb="00999999"/>
+        <fgColor rgb="001E90FF"/>
+        <bgColor rgb="001E90FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF4500"/>
+        <bgColor rgb="00FF4500"/>
       </patternFill>
     </fill>
     <fill>
@@ -62,7 +72,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,28 +80,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1" justifyLastLine="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1" justifyLastLine="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1" justifyLastLine="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1" justifyLastLine="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1" justifyLastLine="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1" justifyLastLine="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -487,7 +523,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,7 +554,7 @@
       <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Projekt: 
-Datum: 28.07.2024</t>
+Datum: 29.07.2024</t>
         </is>
       </c>
     </row>
@@ -557,30 +593,42 @@
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>Název stanice</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">- popis inspekce
-</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr"/>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>
-</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr"/>
+          <t xml:space="preserve">- popis inspekce- popis inspekce- popis inspekce- popis inspekce- popis inspekce- popis inspekce- popis inspekce- popis inspekce
+</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>FH-SC12</t>
+        </is>
+      </c>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 1 (FH-2050)
+kontrolér pro vysokorychlostní kamery FH, 2 jádra, NPN/PNP, 2 kamery
+</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">montážní úchyt kamery FH pro FH-SM
+</t>
+        </is>
+      </c>
       <c r="F4" s="5" t="inlineStr">
         <is>
-          <t>
-</t>
-        </is>
-      </c>
-      <c r="G4" s="4" t="inlineStr">
+          <t xml:space="preserve">Alternativa: 3Z4S-LE SV-3514H
+Objektiv: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 25 mm, nejmenší vzdálenost 150mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+Alternativní: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 25 mm, nejmenší vzdálenost 150mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+</t>
+        </is>
+      </c>
+      <c r="G4" s="8" t="inlineStr">
         <is>
           <t>FH-2050</t>
         </is>
@@ -588,34 +636,670 @@
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">Kontroler 1 (FH-2050)
-</t>
-        </is>
-      </c>
-      <c r="I4" s="4" t="inlineStr"/>
-      <c r="J4" s="4" t="inlineStr"/>
+kontrolér pro vysokorychlostní kamery FH, 2 jádra, NPN/PNP, 2 kamery
+</t>
+        </is>
+      </c>
+      <c r="I4" s="6" t="inlineStr">
+        <is>
+          <t>FH-SM-XLC</t>
+        </is>
+      </c>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">montážní úchyt kamery FH pro FH-SM
+</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="n"/>
+      <c r="A5" s="4" t="n"/>
       <c r="B5" s="6" t="n"/>
       <c r="C5" s="6" t="n"/>
       <c r="D5" s="6" t="n"/>
-      <c r="E5" s="6" t="n"/>
-      <c r="F5" s="6" t="n"/>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">montážní úchyt kamery FH pro FH-SM
+</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE SV-3514H
+Alternativní: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 25 mm, nejmenší vzdálenost 150mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+</t>
+        </is>
+      </c>
       <c r="G5" s="6" t="n"/>
       <c r="H5" s="6" t="n"/>
-      <c r="I5" s="6" t="n"/>
-      <c r="J5" s="6" t="n"/>
+      <c r="I5" s="6" t="inlineStr">
+        <is>
+          <t>FH-SM-XLC</t>
+        </is>
+      </c>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">montážní úchyt kamery FH pro FH-SM
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="6" t="n"/>
+      <c r="D6" s="6" t="n"/>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">dotyková obrazovka kamerového systému FH 12"
+</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="6" t="n"/>
+      <c r="H6" s="6" t="n"/>
+      <c r="I6" s="6" t="inlineStr">
+        <is>
+          <t>FH-MT12</t>
+        </is>
+      </c>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">dotyková obrazovka kamerového systému FH 12"
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="6" t="n"/>
+      <c r="D7" s="6" t="n"/>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="6" t="n"/>
+      <c r="H7" s="6" t="n"/>
+      <c r="I7" s="6" t="inlineStr">
+        <is>
+          <t>rozšíření kontroleru</t>
+        </is>
+      </c>
+      <c r="J7" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="n"/>
+      <c r="B8" s="10" t="n"/>
+      <c r="C8" s="10" t="n"/>
+      <c r="D8" s="10" t="n"/>
+      <c r="E8" s="10" t="n"/>
+      <c r="F8" s="10" t="n"/>
+      <c r="G8" s="10" t="n"/>
+      <c r="H8" s="10" t="n"/>
+      <c r="I8" s="10" t="n"/>
+      <c r="J8" s="10" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">22222222222222222
+</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="inlineStr">
+        <is>
+          <t>FH-SM</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 2 (FH-5050-10)
+kontrolér pro vysokorychlostní / vysokovýkonové kamery FH, 4 jádra, NPN/PNP, 4 kamery
+</t>
+        </is>
+      </c>
+      <c r="E9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fdddddddds
+</t>
+        </is>
+      </c>
+      <c r="F9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE SV-2514H
+Objektiv: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 50 mm, nejmenší vzdálenost 300mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+Alternativní: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 16 mm, nejmenší vzdálenost 100mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+</t>
+        </is>
+      </c>
+      <c r="G9" s="6" t="inlineStr">
+        <is>
+          <t>FH-5050-10</t>
+        </is>
+      </c>
+      <c r="H9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 2 (FH-5050-10)
+kontrolér pro vysokorychlostní / vysokovýkonové kamery FH, 4 jádra, NPN/PNP, 4 kamery
+</t>
+        </is>
+      </c>
+      <c r="I9" s="6" t="inlineStr">
+        <is>
+          <t>monitor</t>
+        </is>
+      </c>
+      <c r="J9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fdddddddds
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="6" t="n"/>
+      <c r="C10" s="6" t="n"/>
+      <c r="D10" s="6" t="n"/>
+      <c r="E10" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">adfadfdfadfs
+</t>
+        </is>
+      </c>
+      <c r="F10" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE SV-5014H
+Objektiv: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 75 mm, nejmenší vzdálenost 1200mm, světelnost 2,5 až zavřeno, maximální kompatiblní CCD čip 2/3" nebo 1", revize 1
+Alternativní: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 35 mm, nejmenší vzdálenost 200mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="n"/>
+      <c r="H10" s="6" t="n"/>
+      <c r="I10" s="6" t="inlineStr">
+        <is>
+          <t>FH-MT12</t>
+        </is>
+      </c>
+      <c r="J10" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">adfadfdfadfs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n"/>
+      <c r="B11" s="6" t="n"/>
+      <c r="C11" s="6" t="n"/>
+      <c r="D11" s="6" t="n"/>
+      <c r="E11" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">adsfdffds
+</t>
+        </is>
+      </c>
+      <c r="F11" s="5" t="inlineStr"/>
+      <c r="G11" s="6" t="n"/>
+      <c r="H11" s="6" t="n"/>
+      <c r="I11" s="6" t="inlineStr">
+        <is>
+          <t>konzole</t>
+        </is>
+      </c>
+      <c r="J11" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">adsfdffds
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n"/>
+      <c r="B12" s="6" t="n"/>
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>FH-SM</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 2 (FH-5050-10)
+kontrolér pro vysokorychlostní / vysokovýkonové kamery FH, 4 jádra, NPN/PNP, 4 kamery
+</t>
+        </is>
+      </c>
+      <c r="E12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fdddddddds
+</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE VS-L10028/M42-10
+Objektiv: Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 35 mm, nejmenší vzdálenost 200mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"
+Alternativní: Objektiv, ultra vysoké rozlišení, nízké zkreslení 16 mm pro 1/1" velik
+</t>
+        </is>
+      </c>
+      <c r="G12" s="6" t="inlineStr">
+        <is>
+          <t>FH-5050-10</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 2 (FH-5050-10)
+kontrolér pro vysokorychlostní / vysokovýkonové kamery FH, 4 jádra, NPN/PNP, 4 kamery
+</t>
+        </is>
+      </c>
+      <c r="I12" s="6" t="inlineStr">
+        <is>
+          <t>monitor</t>
+        </is>
+      </c>
+      <c r="J12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fdddddddds
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n"/>
+      <c r="B13" s="6" t="n"/>
+      <c r="C13" s="6" t="n"/>
+      <c r="D13" s="6" t="n"/>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">adfadfdfadfs
+</t>
+        </is>
+      </c>
+      <c r="F13" s="5" t="inlineStr"/>
+      <c r="G13" s="6" t="n"/>
+      <c r="H13" s="6" t="n"/>
+      <c r="I13" s="6" t="inlineStr">
+        <is>
+          <t>FH-MT12</t>
+        </is>
+      </c>
+      <c r="J13" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">adfadfdfadfs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n"/>
+      <c r="B14" s="6" t="n"/>
+      <c r="C14" s="6" t="n"/>
+      <c r="D14" s="6" t="n"/>
+      <c r="E14" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">adsfdffds
+</t>
+        </is>
+      </c>
+      <c r="F14" s="5" t="inlineStr"/>
+      <c r="G14" s="6" t="n"/>
+      <c r="H14" s="6" t="n"/>
+      <c r="I14" s="6" t="inlineStr">
+        <is>
+          <t>konzole</t>
+        </is>
+      </c>
+      <c r="J14" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">adsfdffds
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="9" t="n"/>
+      <c r="B15" s="10" t="n"/>
+      <c r="C15" s="10" t="n"/>
+      <c r="D15" s="10" t="n"/>
+      <c r="E15" s="10" t="n"/>
+      <c r="F15" s="10" t="n"/>
+      <c r="G15" s="10" t="n"/>
+      <c r="H15" s="10" t="n"/>
+      <c r="I15" s="10" t="n"/>
+      <c r="J15" s="10" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- popis inspekce- popis inspekce- popis inspekce- popis inspekce
+</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>FH-SCX05</t>
+        </is>
+      </c>
+      <c r="D16" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 3 (FH-2050)
+</t>
+        </is>
+      </c>
+      <c r="E16" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="F16" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE VS-HVA3522
+Objektiv: Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 50 mm
+Alternativní: Příslušenství pro kamery, pro M42-montáž, prodlužovací kroužek, sada 5 kroužků (20, 10, 8, 2, 1 mm)
+</t>
+        </is>
+      </c>
+      <c r="G16" s="12" t="inlineStr">
+        <is>
+          <t>FH-2050</t>
+        </is>
+      </c>
+      <c r="H16" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 3 (FH-2050)
+</t>
+        </is>
+      </c>
+      <c r="I16" s="6" t="inlineStr">
+        <is>
+          <t>kabel ke kameře</t>
+        </is>
+      </c>
+      <c r="J16" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n"/>
+      <c r="B17" s="6" t="n"/>
+      <c r="C17" s="6" t="n"/>
+      <c r="D17" s="6" t="n"/>
+      <c r="E17" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="F17" s="5" t="inlineStr"/>
+      <c r="G17" s="6" t="n"/>
+      <c r="H17" s="6" t="n"/>
+      <c r="I17" s="6" t="inlineStr">
+        <is>
+          <t>kamera</t>
+        </is>
+      </c>
+      <c r="J17" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="n"/>
+      <c r="B18" s="10" t="n"/>
+      <c r="C18" s="10" t="n"/>
+      <c r="D18" s="10" t="n"/>
+      <c r="E18" s="10" t="n"/>
+      <c r="F18" s="10" t="n"/>
+      <c r="G18" s="10" t="n"/>
+      <c r="H18" s="10" t="n"/>
+      <c r="I18" s="10" t="n"/>
+      <c r="J18" s="10" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
+          <t>Název staniceghggg</t>
+        </is>
+      </c>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- popis inspekce
+</t>
+        </is>
+      </c>
+      <c r="C19" s="6" t="inlineStr"/>
+      <c r="D19" s="6" t="inlineStr"/>
+      <c r="E19" s="6" t="n"/>
+      <c r="F19" s="6" t="n"/>
+      <c r="G19" s="6" t="n"/>
+      <c r="H19" s="6" t="n"/>
+      <c r="I19" s="6" t="n"/>
+      <c r="J19" s="6" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="9" t="n"/>
+      <c r="B20" s="10" t="n"/>
+      <c r="C20" s="10" t="n"/>
+      <c r="D20" s="10" t="n"/>
+      <c r="E20" s="10" t="n"/>
+      <c r="F20" s="10" t="n"/>
+      <c r="G20" s="10" t="n"/>
+      <c r="H20" s="10" t="n"/>
+      <c r="I20" s="10" t="n"/>
+      <c r="J20" s="10" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>Název stanice</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- popis inspekce
+</t>
+        </is>
+      </c>
+      <c r="C21" s="6" t="inlineStr">
+        <is>
+          <t>FH-SCX01</t>
+        </is>
+      </c>
+      <c r="D21" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 1 (FH-2050)
+kontrolér pro vysokorychlostní kamery FH, 2 jádra, NPN/PNP, 2 kamery
+</t>
+        </is>
+      </c>
+      <c r="E21" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">montážní úchyt kamery FH pro FH-SM
+</t>
+        </is>
+      </c>
+      <c r="F21" s="5" t="inlineStr"/>
+      <c r="G21" s="8" t="inlineStr">
+        <is>
+          <t>FH-2050</t>
+        </is>
+      </c>
+      <c r="H21" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler 1 (FH-2050)
+kontrolér pro vysokorychlostní kamery FH, 2 jádra, NPN/PNP, 2 kamery
+</t>
+        </is>
+      </c>
+      <c r="I21" s="6" t="inlineStr">
+        <is>
+          <t>FH-SM-XLC</t>
+        </is>
+      </c>
+      <c r="J21" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">montážní úchyt kamery FH pro FH-SM
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="n"/>
+      <c r="B22" s="6" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="6" t="n"/>
+      <c r="E22" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">montážní úchyt kamery FH pro FH-SM
+</t>
+        </is>
+      </c>
+      <c r="F22" s="5" t="inlineStr"/>
+      <c r="G22" s="6" t="n"/>
+      <c r="H22" s="6" t="n"/>
+      <c r="I22" s="6" t="inlineStr">
+        <is>
+          <t>FH-SM-XLC</t>
+        </is>
+      </c>
+      <c r="J22" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">montážní úchyt kamery FH pro FH-SM
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="n"/>
+      <c r="B23" s="6" t="n"/>
+      <c r="C23" s="6" t="n"/>
+      <c r="D23" s="6" t="n"/>
+      <c r="E23" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">dotyková obrazovka kamerového systému FH 12"
+</t>
+        </is>
+      </c>
+      <c r="F23" s="5" t="inlineStr"/>
+      <c r="G23" s="6" t="n"/>
+      <c r="H23" s="6" t="n"/>
+      <c r="I23" s="6" t="inlineStr">
+        <is>
+          <t>FH-MT12</t>
+        </is>
+      </c>
+      <c r="J23" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">dotyková obrazovka kamerového systému FH 12"
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="n"/>
+      <c r="B24" s="6" t="n"/>
+      <c r="C24" s="6" t="n"/>
+      <c r="D24" s="6" t="n"/>
+      <c r="E24" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="F24" s="5" t="inlineStr"/>
+      <c r="G24" s="6" t="n"/>
+      <c r="H24" s="6" t="n"/>
+      <c r="I24" s="6" t="inlineStr">
+        <is>
+          <t>rozšíření kontroleru</t>
+        </is>
+      </c>
+      <c r="J24" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9" t="n"/>
+      <c r="B25" s="10" t="n"/>
+      <c r="C25" s="10" t="n"/>
+      <c r="D25" s="10" t="n"/>
+      <c r="E25" s="10" t="n"/>
+      <c r="F25" s="10" t="n"/>
+      <c r="G25" s="10" t="n"/>
+      <c r="H25" s="10" t="n"/>
+      <c r="I25" s="10" t="n"/>
+      <c r="J25" s="10" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:A2"/>
+  <mergeCells count="36">
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="B21:B24"/>
     <mergeCell ref="B1:J1"/>
-    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H21:H24"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C21:C24"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C9:C11"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B2:J2"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
dodělani controller duplicit, offline excel db, práce na loadingu
</commit_message>
<xml_diff>
--- a/TRIMAZKON/Katalog_kamerového_vybavení.xlsx
+++ b/TRIMAZKON/Katalog_kamerového_vybavení.xlsx
@@ -501,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,7 +563,7 @@
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>24.06.2025</t>
+          <t>07.08.2025</t>
         </is>
       </c>
     </row>
@@ -599,25 +599,23 @@
       </c>
       <c r="J5" s="5" t="n"/>
     </row>
-    <row r="6" ht="45" customHeight="1">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="6" t="inlineStr"/>
       <c r="B6" s="7" t="inlineStr"/>
       <c r="C6" s="7" t="inlineStr">
         <is>
-          <t>FH-SM05R</t>
-        </is>
-      </c>
-      <c r="D6" s="7" t="inlineStr">
-        <is>
-          <t>Příslušenství ke kameře:
-3G3RV-PFI3018-SE</t>
-        </is>
-      </c>
-      <c r="E6" s="7" t="inlineStr"/>
+          <t>FHV7H-C016-C</t>
+        </is>
+      </c>
+      <c r="D6" s="7" t="inlineStr"/>
+      <c r="E6" s="7" t="inlineStr">
+        <is>
+          <t>K50RPLPGREQP</t>
+        </is>
+      </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
-          <t>Příslušenství k optice:
-FHV-XMT-7</t>
+          <t>Alternativa: FZ-LEH50</t>
         </is>
       </c>
       <c r="G6" s="7" t="n"/>
@@ -626,67 +624,25 @@
       <c r="J6" s="7" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="n"/>
-      <c r="B7" s="7" t="n"/>
-      <c r="C7" s="7" t="n"/>
-      <c r="D7" s="7" t="n"/>
-      <c r="E7" s="7" t="inlineStr">
-        <is>
-          <t>3Z4S-LE SV-1614H</t>
-        </is>
-      </c>
-      <c r="F7" s="7" t="inlineStr">
-        <is>
-          <t>Objektiv - popis: Objektiv 16 mm</t>
-        </is>
-      </c>
-      <c r="G7" s="7" t="n"/>
-      <c r="H7" s="7" t="n"/>
-      <c r="I7" s="7" t="n"/>
-      <c r="J7" s="7" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="n"/>
-      <c r="B8" s="7" t="n"/>
-      <c r="C8" s="7" t="inlineStr">
-        <is>
-          <t>FH-SM05R</t>
-        </is>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="n"/>
-      <c r="H8" s="7" t="n"/>
-      <c r="I8" s="7" t="n"/>
-      <c r="J8" s="7" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="8" t="n"/>
-      <c r="B9" s="8" t="n"/>
-      <c r="C9" s="8" t="n"/>
-      <c r="D9" s="8" t="n"/>
-      <c r="E9" s="8" t="n"/>
-      <c r="F9" s="8" t="n"/>
-      <c r="G9" s="8" t="n"/>
-      <c r="H9" s="8" t="n"/>
-      <c r="I9" s="8" t="n"/>
-      <c r="J9" s="8" t="n"/>
+      <c r="A7" s="8" t="n"/>
+      <c r="B7" s="8" t="n"/>
+      <c r="C7" s="8" t="n"/>
+      <c r="D7" s="8" t="n"/>
+      <c r="E7" s="8" t="n"/>
+      <c r="F7" s="8" t="n"/>
+      <c r="G7" s="8" t="n"/>
+      <c r="H7" s="8" t="n"/>
+      <c r="I7" s="8" t="n"/>
+      <c r="J7" s="8" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="7">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
     <mergeCell ref="B1:C3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -700,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -802,36 +758,18 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>FH-SM05R</t>
+          <t>FHV7H-C016-C</t>
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>3Z4S-LE SV-1614H</t>
+          <t>K50RPLPGREQP</t>
         </is>
       </c>
       <c r="E3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="inlineStr">
-        <is>
-          <t>3G3RV-PFI3018-SE</t>
-        </is>
-      </c>
-      <c r="N3" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="M4" s="1" t="inlineStr">
-        <is>
-          <t>FHV-XMT-7</t>
-        </is>
-      </c>
-      <c r="N4" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>